<commit_message>
v9.8 Animations in all pages
</commit_message>
<xml_diff>
--- a/src/main/resources/NutrititionalPlanRules.xlsx
+++ b/src/main/resources/NutrititionalPlanRules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{713138D4-F576-4897-A509-E344C13D3C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5C149761-071E-48EF-A9DB-EAC14D39C427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -762,8 +762,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A5" sqref="A5"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>